<commit_message>
unet vgg16 bn experiment complete
</commit_message>
<xml_diff>
--- a/Experiments/Experiments.xlsx
+++ b/Experiments/Experiments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Backbone</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>resnet18</t>
+  </si>
+  <si>
+    <t>vgg16_bn</t>
   </si>
 </sst>
 </file>
@@ -208,6 +214,158 @@
         <a:xfrm>
           <a:off x="6659880" y="586741"/>
           <a:ext cx="2232660" cy="1638299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>777393</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>62345</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>278755</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>115454</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1385454" y="3017981"/>
+          <a:ext cx="2318453" cy="1715655"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>429128</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>46182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>737585</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>107757</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6663673" y="3001818"/>
+          <a:ext cx="2317367" cy="1724121"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>708122</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>130850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>246303</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>46505</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1316183" y="5857395"/>
+          <a:ext cx="2355272" cy="1762928"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>439609</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>7697</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>792787</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>24952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6674154" y="5918970"/>
+          <a:ext cx="2362088" cy="1679800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -482,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="99" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,6 +738,88 @@
         <v>18</v>
       </c>
     </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14">
+        <v>1E-4</v>
+      </c>
+      <c r="H14">
+        <v>75</v>
+      </c>
+      <c r="I14">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J14">
+        <v>0.18</v>
+      </c>
+      <c r="K14">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="L14">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="M14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28">
+        <v>1E-4</v>
+      </c>
+      <c r="H28">
+        <v>75</v>
+      </c>
+      <c r="I28">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J28">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="K28">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="L28">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="M28" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
unet vgg16 bn augmentation experiment done
</commit_message>
<xml_diff>
--- a/Experiments/Experiments.xlsx
+++ b/Experiments/Experiments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Backbone</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>vgg16_bn</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>FPN</t>
+  </si>
+  <si>
+    <t>Unet</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -148,13 +160,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>723901</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>45721</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>106681</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
@@ -186,14 +198,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>647701</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
@@ -224,13 +236,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>777393</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>62345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>278755</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>115454</xdr:rowOff>
@@ -262,14 +274,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>429128</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>46182</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>737585</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>737586</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>107757</xdr:rowOff>
     </xdr:to>
@@ -300,13 +312,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>708122</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>130850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>246303</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>46505</xdr:rowOff>
@@ -338,14 +350,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>439609</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>7697</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>792787</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>792788</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>24952</xdr:rowOff>
     </xdr:to>
@@ -366,6 +378,82 @@
         <a:xfrm>
           <a:off x="6674154" y="5918970"/>
           <a:ext cx="2362088" cy="1679800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>481936</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>131883</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>461038</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>161193</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1698205" y="8557845"/>
+          <a:ext cx="2792641" cy="2044213"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>327499</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>139212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>183232</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7163518" y="8565174"/>
+          <a:ext cx="2874426" cy="2058864"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -640,184 +728,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="104" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1E-4</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>75</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.19</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.96</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.72299999999999998</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>13</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>17</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>15</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>1E-4</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>75</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.18</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>0.95199999999999996</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>0.73499999999999999</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
       <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
         <v>20</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>12</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>13</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>17</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>15</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>1E-4</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>75</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>0.17699999999999999</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>0.96499999999999997</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>0.73799999999999999</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44">
+        <v>1E-4</v>
+      </c>
+      <c r="I44">
+        <v>40</v>
+      </c>
+      <c r="J44">
+        <v>0.106</v>
+      </c>
+      <c r="K44">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="L44">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="M44">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="N44" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>